<commit_message>
Add old holder saving
</commit_message>
<xml_diff>
--- a/whales/holders.xlsx
+++ b/whales/holders.xlsx
@@ -512,7 +512,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>761,162,863,019,330</t>
+          <t>761,164,086,613,816</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
@@ -1853,7 +1853,7 @@
       </c>
       <c r="C51" s="3" t="inlineStr">
         <is>
-          <t>12,000,523,943,691,467</t>
+          <t>12,000,525,167,285,953</t>
         </is>
       </c>
       <c r="D51" s="3" t="inlineStr">
@@ -1896,32 +1896,32 @@
       </c>
       <c r="B54" s="4" t="inlineStr">
         <is>
-          <t>0x505dd22c1bacced7531f319f5008318a440490bc</t>
+          <t>0x2bd6997bf6fcfde139eb1b9346fbf79defd4e8cc</t>
         </is>
       </c>
       <c r="C54" s="5" t="inlineStr">
         <is>
-          <t>90,055,783,444,045</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D54" s="5" t="inlineStr">
         <is>
-          <t>90 Trillion</t>
+          <t>0 Trillion</t>
         </is>
       </c>
       <c r="E54" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.0950% </t>
+          <t xml:space="preserve">0.5497% </t>
         </is>
       </c>
       <c r="F54" s="6" t="inlineStr">
         <is>
-          <t>5 Trillion Less</t>
+          <t>550 Trillion Less</t>
         </is>
       </c>
       <c r="G54" s="7" t="inlineStr">
         <is>
-          <t>4,948,463,529,878</t>
+          <t>549,662,717,019,826</t>
         </is>
       </c>
     </row>
@@ -1931,32 +1931,32 @@
       </c>
       <c r="B55" s="4" t="inlineStr">
         <is>
-          <t>0x3d268cd580f89cfe6cc5dcf8764f51085f74a649</t>
+          <t>0x505dd22c1bacced7531f319f5008318a440490bc</t>
         </is>
       </c>
       <c r="C55" s="5" t="inlineStr">
         <is>
-          <t>4,788,212,804,945</t>
+          <t>90,056,129,846,728</t>
         </is>
       </c>
       <c r="D55" s="5" t="inlineStr">
         <is>
-          <t>5 Trillion</t>
+          <t>90 Trillion</t>
         </is>
       </c>
       <c r="E55" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1278% </t>
+          <t xml:space="preserve">0.0950% </t>
         </is>
       </c>
       <c r="F55" s="6" t="inlineStr">
         <is>
-          <t>123 Trillion Less</t>
+          <t>5 Trillion Less</t>
         </is>
       </c>
       <c r="G55" s="7" t="inlineStr">
         <is>
-          <t>123,043,254,976,892</t>
+          <t>4,948,117,127,195</t>
         </is>
       </c>
     </row>
@@ -1966,32 +1966,32 @@
       </c>
       <c r="B56" s="4" t="inlineStr">
         <is>
-          <t>0x2bd6997bf6fcfde139eb1b9346fbf79defd4e8cc</t>
+          <t>0x3d268cd580f89cfe6cc5dcf8764f51085f74a649</t>
         </is>
       </c>
       <c r="C56" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>4,788,231,222,971</t>
         </is>
       </c>
       <c r="D56" s="5" t="inlineStr">
         <is>
-          <t>0 Trillion</t>
+          <t>5 Trillion</t>
         </is>
       </c>
       <c r="E56" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.5497% </t>
+          <t xml:space="preserve">0.1278% </t>
         </is>
       </c>
       <c r="F56" s="6" t="inlineStr">
         <is>
-          <t>550 Trillion Less</t>
+          <t>123 Trillion Less</t>
         </is>
       </c>
       <c r="G56" s="7" t="inlineStr">
         <is>
-          <t>549,662,717,019,826</t>
+          <t>123,043,236,558,866</t>
         </is>
       </c>
     </row>
@@ -2009,7 +2009,7 @@
       </c>
       <c r="G58" s="6" t="inlineStr">
         <is>
-          <t>-709,084,111,067,757</t>
+          <t>-709,083,746,247,048</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
My oh my it's another update
</commit_message>
<xml_diff>
--- a/whales/holders.xlsx
+++ b/whales/holders.xlsx
@@ -451,7 +451,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,7 +512,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>773,966,741,108,558</t>
+          <t>774,216,186,127,082</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
@@ -522,7 +522,7 @@
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.7740% </t>
+          <t xml:space="preserve">0.7742% </t>
         </is>
       </c>
       <c r="F2" s="2" t="n"/>
@@ -539,17 +539,17 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>608,453,920,837,053</t>
+          <t>608,650,037,852,732</t>
         </is>
       </c>
       <c r="D3" s="3" t="inlineStr">
         <is>
-          <t>608 Trillion</t>
+          <t>609 Trillion</t>
         </is>
       </c>
       <c r="E3" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.6085% </t>
+          <t xml:space="preserve">0.6087% </t>
         </is>
       </c>
       <c r="F3" s="2" t="n"/>
@@ -566,7 +566,7 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>410,958,271,336,168</t>
+          <t>411,090,731,506,089</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
@@ -576,7 +576,7 @@
       </c>
       <c r="E4" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.4110% </t>
+          <t xml:space="preserve">0.4111% </t>
         </is>
       </c>
       <c r="F4" s="2" t="n"/>
@@ -593,7 +593,7 @@
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>409,310,791,675,035</t>
+          <t>409,442,720,828,911</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
@@ -603,7 +603,7 @@
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.4093% </t>
+          <t xml:space="preserve">0.4094% </t>
         </is>
       </c>
       <c r="F5" s="2" t="n"/>
@@ -620,7 +620,7 @@
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>401,861,671,278,250</t>
+          <t>401,991,199,429,829</t>
         </is>
       </c>
       <c r="D6" s="3" t="inlineStr">
@@ -630,7 +630,7 @@
       </c>
       <c r="E6" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.4019% </t>
+          <t xml:space="preserve">0.4020% </t>
         </is>
       </c>
       <c r="F6" s="2" t="n"/>
@@ -647,7 +647,7 @@
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>387,751,635,218,310</t>
+          <t>387,893,772,035,584</t>
         </is>
       </c>
       <c r="D7" s="5" t="inlineStr">
@@ -657,7 +657,7 @@
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.3878% </t>
+          <t xml:space="preserve">0.3879% </t>
         </is>
       </c>
       <c r="F7" s="6" t="inlineStr">
@@ -667,7 +667,7 @@
       </c>
       <c r="G7" s="7" t="inlineStr">
         <is>
-          <t>30,125,647,999,106</t>
+          <t>29,983,511,181,832</t>
         </is>
       </c>
     </row>
@@ -682,7 +682,7 @@
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>375,018,721,635,353</t>
+          <t>375,131,643,268,213</t>
         </is>
       </c>
       <c r="D8" s="3" t="inlineStr">
@@ -692,7 +692,7 @@
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.3750% </t>
+          <t xml:space="preserve">0.3751% </t>
         </is>
       </c>
       <c r="F8" s="2" t="n"/>
@@ -709,27 +709,27 @@
       </c>
       <c r="C9" s="5" t="inlineStr">
         <is>
-          <t>311,389,968,724,782</t>
+          <t>316,311,829,818,156</t>
         </is>
       </c>
       <c r="D9" s="5" t="inlineStr">
         <is>
-          <t>311 Trillion</t>
+          <t>316 Trillion</t>
         </is>
       </c>
       <c r="E9" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.3114% </t>
+          <t xml:space="preserve">0.3163% </t>
         </is>
       </c>
       <c r="F9" s="4" t="inlineStr">
         <is>
-          <t>5 Trillion More</t>
+          <t>10 Trillion More</t>
         </is>
       </c>
       <c r="G9" s="5" t="inlineStr">
         <is>
-          <t>5,010,226,110,545</t>
+          <t>9,932,087,203,919</t>
         </is>
       </c>
     </row>
@@ -806,7 +806,7 @@
       </c>
       <c r="C12" s="5" t="inlineStr">
         <is>
-          <t>200,241,335,294,152</t>
+          <t>200,307,986,170,445</t>
         </is>
       </c>
       <c r="D12" s="5" t="inlineStr">
@@ -816,7 +816,7 @@
       </c>
       <c r="E12" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.2002% </t>
+          <t xml:space="preserve">0.2003% </t>
         </is>
       </c>
       <c r="F12" s="4" t="inlineStr">
@@ -826,7 +826,7 @@
       </c>
       <c r="G12" s="5" t="inlineStr">
         <is>
-          <t>14,194,480,143,751</t>
+          <t>14,261,131,020,044</t>
         </is>
       </c>
     </row>
@@ -836,22 +836,22 @@
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>0x7146f34d166379b4ab5220f5eefd7c79835a3c04</t>
+          <t>0x573068628665a40aa2dddfd5ec3c90167424a9ee</t>
         </is>
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>196,911,442,860,571</t>
+          <t>190,593,752,012,968</t>
         </is>
       </c>
       <c r="D13" s="3" t="inlineStr">
         <is>
-          <t>197 Trillion</t>
+          <t>191 Trillion</t>
         </is>
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1969% </t>
+          <t xml:space="preserve">0.1906% </t>
         </is>
       </c>
       <c r="F13" s="2" t="n"/>
@@ -863,53 +863,61 @@
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>0x573068628665a40aa2dddfd5ec3c90167424a9ee</t>
+          <t>0x73149b3cd5e1b8536747048259419147e81a71a9</t>
         </is>
       </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>190,593,752,012,968</t>
+          <t>188,093,487,682,416</t>
         </is>
       </c>
       <c r="D14" s="3" t="inlineStr">
         <is>
-          <t>191 Trillion</t>
+          <t>188 Trillion</t>
         </is>
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1906% </t>
+          <t xml:space="preserve">0.1881% </t>
         </is>
       </c>
       <c r="F14" s="2" t="n"/>
       <c r="G14" s="2" t="n"/>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="n">
+      <c r="A15" s="4" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="inlineStr">
-        <is>
-          <t>0x73149b3cd5e1b8536747048259419147e81a71a9</t>
-        </is>
-      </c>
-      <c r="C15" s="3" t="inlineStr">
-        <is>
-          <t>188,093,487,682,416</t>
-        </is>
-      </c>
-      <c r="D15" s="3" t="inlineStr">
-        <is>
-          <t>188 Trillion</t>
-        </is>
-      </c>
-      <c r="E15" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.1881% </t>
-        </is>
-      </c>
-      <c r="F15" s="2" t="n"/>
-      <c r="G15" s="2" t="n"/>
+      <c r="B15" s="4" t="inlineStr">
+        <is>
+          <t>0x7146f34d166379b4ab5220f5eefd7c79835a3c04</t>
+        </is>
+      </c>
+      <c r="C15" s="5" t="inlineStr">
+        <is>
+          <t>180,049,748,547,878</t>
+        </is>
+      </c>
+      <c r="D15" s="5" t="inlineStr">
+        <is>
+          <t>180 Trillion</t>
+        </is>
+      </c>
+      <c r="E15" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.1800% </t>
+        </is>
+      </c>
+      <c r="F15" s="6" t="inlineStr">
+        <is>
+          <t>17 Trillion Less</t>
+        </is>
+      </c>
+      <c r="G15" s="7" t="inlineStr">
+        <is>
+          <t>16,708,711,049,687</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
@@ -922,7 +930,7 @@
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>174,345,288,488,457</t>
+          <t>174,420,634,860,359</t>
         </is>
       </c>
       <c r="D16" s="3" t="inlineStr">
@@ -932,7 +940,7 @@
       </c>
       <c r="E16" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1743% </t>
+          <t xml:space="preserve">0.1744% </t>
         </is>
       </c>
       <c r="F16" s="2" t="n"/>
@@ -949,7 +957,7 @@
       </c>
       <c r="C17" s="3" t="inlineStr">
         <is>
-          <t>171,873,113,601,026</t>
+          <t>171,919,094,110,735</t>
         </is>
       </c>
       <c r="D17" s="3" t="inlineStr">
@@ -976,12 +984,12 @@
       </c>
       <c r="C18" s="5" t="inlineStr">
         <is>
-          <t>161,467,210,436,966</t>
+          <t>161,527,403,951,616</t>
         </is>
       </c>
       <c r="D18" s="5" t="inlineStr">
         <is>
-          <t>161 Trillion</t>
+          <t>162 Trillion</t>
         </is>
       </c>
       <c r="E18" s="5" t="inlineStr">
@@ -996,7 +1004,7 @@
       </c>
       <c r="G18" s="5" t="inlineStr">
         <is>
-          <t>50,949,114,342,863</t>
+          <t>51,009,307,857,513</t>
         </is>
       </c>
     </row>
@@ -1038,7 +1046,7 @@
       </c>
       <c r="C20" s="3" t="inlineStr">
         <is>
-          <t>153,573,565,770,106</t>
+          <t>153,700,859,113,465</t>
         </is>
       </c>
       <c r="D20" s="3" t="inlineStr">
@@ -1048,7 +1056,7 @@
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1536% </t>
+          <t xml:space="preserve">0.1537% </t>
         </is>
       </c>
       <c r="F20" s="2" t="n"/>
@@ -1065,7 +1073,7 @@
       </c>
       <c r="C21" s="5" t="inlineStr">
         <is>
-          <t>151,299,609,473,015</t>
+          <t>151,329,188,545,567</t>
         </is>
       </c>
       <c r="D21" s="5" t="inlineStr">
@@ -1085,36 +1093,44 @@
       </c>
       <c r="G21" s="7" t="inlineStr">
         <is>
-          <t>28,749,897,594,216</t>
+          <t>28,720,318,521,664</t>
         </is>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="2" t="n">
+      <c r="A22" s="4" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="2" t="inlineStr">
-        <is>
-          <t>0xf08ae27b3b1c31d1cfc2879e2ae567d81d42bdeb</t>
-        </is>
-      </c>
-      <c r="C22" s="3" t="inlineStr">
-        <is>
-          <t>146,080,408,921,801</t>
-        </is>
-      </c>
-      <c r="D22" s="3" t="inlineStr">
-        <is>
-          <t>146 Trillion</t>
-        </is>
-      </c>
-      <c r="E22" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.1461% </t>
-        </is>
-      </c>
-      <c r="F22" s="2" t="n"/>
-      <c r="G22" s="2" t="n"/>
+      <c r="B22" s="4" t="inlineStr">
+        <is>
+          <t>0x4ac84bbb674f62614626f6276296014f1cade575</t>
+        </is>
+      </c>
+      <c r="C22" s="5" t="inlineStr">
+        <is>
+          <t>148,109,255,191,595</t>
+        </is>
+      </c>
+      <c r="D22" s="5" t="inlineStr">
+        <is>
+          <t>148 Trillion</t>
+        </is>
+      </c>
+      <c r="E22" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.1481% </t>
+        </is>
+      </c>
+      <c r="F22" s="4" t="inlineStr">
+        <is>
+          <t>7 Trillion More</t>
+        </is>
+      </c>
+      <c r="G22" s="5" t="inlineStr">
+        <is>
+          <t>6,846,266,779,468</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
@@ -1122,22 +1138,22 @@
       </c>
       <c r="B23" s="2" t="inlineStr">
         <is>
-          <t>0x4ac84bbb674f62614626f6276296014f1cade575</t>
+          <t>0xf08ae27b3b1c31d1cfc2879e2ae567d81d42bdeb</t>
         </is>
       </c>
       <c r="C23" s="3" t="inlineStr">
         <is>
-          <t>141,375,801,302,018</t>
+          <t>146,185,236,267,846</t>
         </is>
       </c>
       <c r="D23" s="3" t="inlineStr">
         <is>
-          <t>141 Trillion</t>
+          <t>146 Trillion</t>
         </is>
       </c>
       <c r="E23" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1414% </t>
+          <t xml:space="preserve">0.1462% </t>
         </is>
       </c>
       <c r="F23" s="2" t="n"/>
@@ -1171,58 +1187,74 @@
       <c r="G24" s="2" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="2" t="n">
+      <c r="A25" s="4" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="2" t="inlineStr">
-        <is>
-          <t>0xf076f6f942eac10b48cea9ed1f25be813304ae42</t>
-        </is>
-      </c>
-      <c r="C25" s="3" t="inlineStr">
-        <is>
-          <t>117,805,227,381,517</t>
-        </is>
-      </c>
-      <c r="D25" s="3" t="inlineStr">
-        <is>
-          <t>118 Trillion</t>
-        </is>
-      </c>
-      <c r="E25" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.1178% </t>
-        </is>
-      </c>
-      <c r="F25" s="2" t="n"/>
-      <c r="G25" s="2" t="n"/>
+      <c r="B25" s="4" t="inlineStr">
+        <is>
+          <t>0x74beaeb59500b4486ec3c83b81552279b79c6728</t>
+        </is>
+      </c>
+      <c r="C25" s="5" t="inlineStr">
+        <is>
+          <t>134,413,919,604,666</t>
+        </is>
+      </c>
+      <c r="D25" s="5" t="inlineStr">
+        <is>
+          <t>134 Trillion</t>
+        </is>
+      </c>
+      <c r="E25" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.1344% </t>
+        </is>
+      </c>
+      <c r="F25" s="4" t="inlineStr">
+        <is>
+          <t>26 Trillion More</t>
+        </is>
+      </c>
+      <c r="G25" s="5" t="inlineStr">
+        <is>
+          <t>26,371,433,221,782</t>
+        </is>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" s="2" t="n">
+      <c r="A26" s="4" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="2" t="inlineStr">
-        <is>
-          <t>0x28e87335c43b9b28d658b6825811744c251f5974</t>
-        </is>
-      </c>
-      <c r="C26" s="3" t="inlineStr">
-        <is>
-          <t>115,222,802,654,107</t>
-        </is>
-      </c>
-      <c r="D26" s="3" t="inlineStr">
-        <is>
-          <t>115 Trillion</t>
-        </is>
-      </c>
-      <c r="E26" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.1152% </t>
-        </is>
-      </c>
-      <c r="F26" s="2" t="n"/>
-      <c r="G26" s="2" t="n"/>
+      <c r="B26" s="4" t="inlineStr">
+        <is>
+          <t>0xf4eaa3a2eb5e8e654eabc030f4395062fe597db3</t>
+        </is>
+      </c>
+      <c r="C26" s="5" t="inlineStr">
+        <is>
+          <t>132,858,715,897,236</t>
+        </is>
+      </c>
+      <c r="D26" s="5" t="inlineStr">
+        <is>
+          <t>133 Trillion</t>
+        </is>
+      </c>
+      <c r="E26" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.1329% </t>
+        </is>
+      </c>
+      <c r="F26" s="4" t="inlineStr">
+        <is>
+          <t>20 Trillion More</t>
+        </is>
+      </c>
+      <c r="G26" s="5" t="inlineStr">
+        <is>
+          <t>19,760,626,096,690</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
@@ -1230,22 +1262,22 @@
       </c>
       <c r="B27" s="2" t="inlineStr">
         <is>
-          <t>0xf4eaa3a2eb5e8e654eabc030f4395062fe597db3</t>
+          <t>0xf076f6f942eac10b48cea9ed1f25be813304ae42</t>
         </is>
       </c>
       <c r="C27" s="3" t="inlineStr">
         <is>
-          <t>113,098,089,800,546</t>
+          <t>117,805,227,381,517</t>
         </is>
       </c>
       <c r="D27" s="3" t="inlineStr">
         <is>
-          <t>113 Trillion</t>
+          <t>118 Trillion</t>
         </is>
       </c>
       <c r="E27" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1131% </t>
+          <t xml:space="preserve">0.1178% </t>
         </is>
       </c>
       <c r="F27" s="2" t="n"/>
@@ -1257,22 +1289,22 @@
       </c>
       <c r="B28" s="2" t="inlineStr">
         <is>
-          <t>0x493d3d63b6e92869098d3ce8d733ce220633b829</t>
+          <t>0x28e87335c43b9b28d658b6825811744c251f5974</t>
         </is>
       </c>
       <c r="C28" s="3" t="inlineStr">
         <is>
-          <t>111,510,350,768,450</t>
+          <t>115,264,502,926,544</t>
         </is>
       </c>
       <c r="D28" s="3" t="inlineStr">
         <is>
-          <t>112 Trillion</t>
+          <t>115 Trillion</t>
         </is>
       </c>
       <c r="E28" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1115% </t>
+          <t xml:space="preserve">0.1153% </t>
         </is>
       </c>
       <c r="F28" s="2" t="n"/>
@@ -1284,88 +1316,88 @@
       </c>
       <c r="B29" s="2" t="inlineStr">
         <is>
-          <t>0xb2c5ae080a236fe89a87fdbd1f9d58ad4b57c6b2</t>
+          <t>0x493d3d63b6e92869098d3ce8d733ce220633b829</t>
         </is>
       </c>
       <c r="C29" s="3" t="inlineStr">
         <is>
-          <t>108,210,934,281,939</t>
+          <t>111,510,350,768,450</t>
         </is>
       </c>
       <c r="D29" s="3" t="inlineStr">
         <is>
-          <t>108 Trillion</t>
+          <t>112 Trillion</t>
         </is>
       </c>
       <c r="E29" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1082% </t>
+          <t xml:space="preserve">0.1115% </t>
         </is>
       </c>
       <c r="F29" s="2" t="n"/>
       <c r="G29" s="2" t="n"/>
     </row>
     <row r="30">
-      <c r="A30" s="4" t="n">
+      <c r="A30" s="2" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="4" t="inlineStr">
+      <c r="B30" s="2" t="inlineStr">
+        <is>
+          <t>0xb2c5ae080a236fe89a87fdbd1f9d58ad4b57c6b2</t>
+        </is>
+      </c>
+      <c r="C30" s="3" t="inlineStr">
+        <is>
+          <t>108,210,934,281,939</t>
+        </is>
+      </c>
+      <c r="D30" s="3" t="inlineStr">
+        <is>
+          <t>108 Trillion</t>
+        </is>
+      </c>
+      <c r="E30" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.1082% </t>
+        </is>
+      </c>
+      <c r="F30" s="2" t="n"/>
+      <c r="G30" s="2" t="n"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="4" t="inlineStr">
         <is>
           <t>0x2fcc0ac77971df25d65b9eae9418434ac72be3bc</t>
         </is>
       </c>
-      <c r="C30" s="5" t="inlineStr">
+      <c r="C31" s="5" t="inlineStr">
         <is>
           <t>108,170,757,830,871</t>
         </is>
       </c>
-      <c r="D30" s="5" t="inlineStr">
+      <c r="D31" s="5" t="inlineStr">
         <is>
           <t>108 Trillion</t>
         </is>
       </c>
-      <c r="E30" s="5" t="inlineStr">
+      <c r="E31" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">0.1082% </t>
         </is>
       </c>
-      <c r="F30" s="4" t="inlineStr">
+      <c r="F31" s="4" t="inlineStr">
         <is>
           <t>6 Trillion More</t>
         </is>
       </c>
-      <c r="G30" s="5" t="inlineStr">
+      <c r="G31" s="5" t="inlineStr">
         <is>
           <t>5,951,202,366,611</t>
         </is>
       </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="2" t="n">
-        <v>30</v>
-      </c>
-      <c r="B31" s="2" t="inlineStr">
-        <is>
-          <t>0xf677ecba7a2a3bfc86fc37ac07ffa2fa896bb525</t>
-        </is>
-      </c>
-      <c r="C31" s="3" t="inlineStr">
-        <is>
-          <t>107,802,445,283,117</t>
-        </is>
-      </c>
-      <c r="D31" s="3" t="inlineStr">
-        <is>
-          <t>108 Trillion</t>
-        </is>
-      </c>
-      <c r="E31" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.1078% </t>
-        </is>
-      </c>
-      <c r="F31" s="2" t="n"/>
-      <c r="G31" s="2" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
@@ -1373,22 +1405,22 @@
       </c>
       <c r="B32" s="2" t="inlineStr">
         <is>
-          <t>0x84d1b0ae25aa0b535552d28455f4d00922baf624</t>
+          <t>0xf677ecba7a2a3bfc86fc37ac07ffa2fa896bb525</t>
         </is>
       </c>
       <c r="C32" s="3" t="inlineStr">
         <is>
-          <t>104,834,199,490,524</t>
+          <t>107,947,760,069,167</t>
         </is>
       </c>
       <c r="D32" s="3" t="inlineStr">
         <is>
-          <t>105 Trillion</t>
+          <t>108 Trillion</t>
         </is>
       </c>
       <c r="E32" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1048% </t>
+          <t xml:space="preserve">0.1079% </t>
         </is>
       </c>
       <c r="F32" s="2" t="n"/>
@@ -1432,7 +1464,7 @@
       </c>
       <c r="C34" s="3" t="inlineStr">
         <is>
-          <t>102,126,985,955,117</t>
+          <t>102,229,246,221,190</t>
         </is>
       </c>
       <c r="D34" s="3" t="inlineStr">
@@ -1442,7 +1474,7 @@
       </c>
       <c r="E34" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1021% </t>
+          <t xml:space="preserve">0.1022% </t>
         </is>
       </c>
       <c r="F34" s="2" t="n"/>
@@ -1508,22 +1540,22 @@
       </c>
       <c r="B37" s="2" t="inlineStr">
         <is>
-          <t>0x69fe97ce030074b37cbaf3ee46e9f68ca8712099</t>
+          <t>0xa9579390b4b5ac986a16a05c32ad0975e089a857</t>
         </is>
       </c>
       <c r="C37" s="3" t="inlineStr">
         <is>
-          <t>100,567,579,913,450</t>
+          <t>100,126,359,859,271</t>
         </is>
       </c>
       <c r="D37" s="3" t="inlineStr">
         <is>
-          <t>101 Trillion</t>
+          <t>100 Trillion</t>
         </is>
       </c>
       <c r="E37" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1006% </t>
+          <t xml:space="preserve">0.1001% </t>
         </is>
       </c>
       <c r="F37" s="2" t="n"/>
@@ -1535,22 +1567,22 @@
       </c>
       <c r="B38" s="2" t="inlineStr">
         <is>
-          <t>0xa9579390b4b5ac986a16a05c32ad0975e089a857</t>
+          <t>0x021bcf7b581b6328c458f13ebb50ea6767c1b16d</t>
         </is>
       </c>
       <c r="C38" s="3" t="inlineStr">
         <is>
-          <t>100,126,359,859,271</t>
+          <t>92,888,524,562,195</t>
         </is>
       </c>
       <c r="D38" s="3" t="inlineStr">
         <is>
-          <t>100 Trillion</t>
+          <t>93 Trillion</t>
         </is>
       </c>
       <c r="E38" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1001% </t>
+          <t xml:space="preserve">0.0929% </t>
         </is>
       </c>
       <c r="F38" s="2" t="n"/>
@@ -1562,22 +1594,22 @@
       </c>
       <c r="B39" s="2" t="inlineStr">
         <is>
-          <t>0x302c44b648f5a84191f08551be26a2d2456a1fa1</t>
+          <t>0xf8a002718fbba65dd1ca19e7027c943c54e20220</t>
         </is>
       </c>
       <c r="C39" s="3" t="inlineStr">
         <is>
-          <t>93,917,447,289,939</t>
+          <t>90,569,119,873,037</t>
         </is>
       </c>
       <c r="D39" s="3" t="inlineStr">
         <is>
-          <t>94 Trillion</t>
+          <t>91 Trillion</t>
         </is>
       </c>
       <c r="E39" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.0939% </t>
+          <t xml:space="preserve">0.0906% </t>
         </is>
       </c>
       <c r="F39" s="2" t="n"/>
@@ -1589,53 +1621,61 @@
       </c>
       <c r="B40" s="2" t="inlineStr">
         <is>
-          <t>0xf8a002718fbba65dd1ca19e7027c943c54e20220</t>
+          <t>0xb501e46d0e187cd9e2e0b3611fe17ed477f998e1</t>
         </is>
       </c>
       <c r="C40" s="3" t="inlineStr">
         <is>
-          <t>90,450,936,429,404</t>
+          <t>87,819,801,364,648</t>
         </is>
       </c>
       <c r="D40" s="3" t="inlineStr">
         <is>
-          <t>90 Trillion</t>
+          <t>88 Trillion</t>
         </is>
       </c>
       <c r="E40" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.0905% </t>
+          <t xml:space="preserve">0.0878% </t>
         </is>
       </c>
       <c r="F40" s="2" t="n"/>
       <c r="G40" s="2" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="2" t="n">
+      <c r="A41" s="4" t="n">
         <v>40</v>
       </c>
-      <c r="B41" s="2" t="inlineStr">
-        <is>
-          <t>0xb501e46d0e187cd9e2e0b3611fe17ed477f998e1</t>
-        </is>
-      </c>
-      <c r="C41" s="3" t="inlineStr">
-        <is>
-          <t>87,819,801,364,648</t>
-        </is>
-      </c>
-      <c r="D41" s="3" t="inlineStr">
-        <is>
-          <t>88 Trillion</t>
-        </is>
-      </c>
-      <c r="E41" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.0878% </t>
-        </is>
-      </c>
-      <c r="F41" s="2" t="n"/>
-      <c r="G41" s="2" t="n"/>
+      <c r="B41" s="4" t="inlineStr">
+        <is>
+          <t>0xd8f8110161649178bca78b074cef0864ad9a99a8</t>
+        </is>
+      </c>
+      <c r="C41" s="5" t="inlineStr">
+        <is>
+          <t>87,159,029,085,616</t>
+        </is>
+      </c>
+      <c r="D41" s="5" t="inlineStr">
+        <is>
+          <t>87 Trillion</t>
+        </is>
+      </c>
+      <c r="E41" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.0872% </t>
+        </is>
+      </c>
+      <c r="F41" s="4" t="inlineStr">
+        <is>
+          <t>4 Trillion More</t>
+        </is>
+      </c>
+      <c r="G41" s="5" t="inlineStr">
+        <is>
+          <t>4,243,865,932,513</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="n">
@@ -1648,7 +1688,7 @@
       </c>
       <c r="C42" s="3" t="inlineStr">
         <is>
-          <t>86,886,701,053,075</t>
+          <t>86,961,842,948,968</t>
         </is>
       </c>
       <c r="D42" s="3" t="inlineStr">
@@ -1658,7 +1698,7 @@
       </c>
       <c r="E42" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.0869% </t>
+          <t xml:space="preserve">0.0870% </t>
         </is>
       </c>
       <c r="F42" s="2" t="n"/>
@@ -1670,22 +1710,22 @@
       </c>
       <c r="B43" s="2" t="inlineStr">
         <is>
-          <t>0x021bcf7b581b6328c458f13ebb50ea6767c1b16d</t>
+          <t>0xa6864e154b64a8ce94020a8c1b43f191d3523c47</t>
         </is>
       </c>
       <c r="C43" s="3" t="inlineStr">
         <is>
-          <t>85,412,639,401,083</t>
+          <t>81,128,791,830,716</t>
         </is>
       </c>
       <c r="D43" s="3" t="inlineStr">
         <is>
-          <t>85 Trillion</t>
+          <t>81 Trillion</t>
         </is>
       </c>
       <c r="E43" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.0854% </t>
+          <t xml:space="preserve">0.0811% </t>
         </is>
       </c>
       <c r="F43" s="2" t="n"/>
@@ -1697,22 +1737,22 @@
       </c>
       <c r="B44" s="2" t="inlineStr">
         <is>
-          <t>0xd8f8110161649178bca78b074cef0864ad9a99a8</t>
+          <t>0x4e57abe60fdc74c47fc3a86bbd7857b4e24c180d</t>
         </is>
       </c>
       <c r="C44" s="3" t="inlineStr">
         <is>
-          <t>82,959,850,141,772</t>
+          <t>79,763,629,301,578</t>
         </is>
       </c>
       <c r="D44" s="3" t="inlineStr">
         <is>
-          <t>83 Trillion</t>
+          <t>80 Trillion</t>
         </is>
       </c>
       <c r="E44" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.0830% </t>
+          <t xml:space="preserve">0.0798% </t>
         </is>
       </c>
       <c r="F44" s="2" t="n"/>
@@ -1724,22 +1764,22 @@
       </c>
       <c r="B45" s="2" t="inlineStr">
         <is>
-          <t>0xa6864e154b64a8ce94020a8c1b43f191d3523c47</t>
+          <t>0xe902fd7de8afb5b295f628c1b4f6143005bb0bf6</t>
         </is>
       </c>
       <c r="C45" s="3" t="inlineStr">
         <is>
-          <t>81,128,791,830,716</t>
+          <t>78,500,122,588,755</t>
         </is>
       </c>
       <c r="D45" s="3" t="inlineStr">
         <is>
-          <t>81 Trillion</t>
+          <t>79 Trillion</t>
         </is>
       </c>
       <c r="E45" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.0811% </t>
+          <t xml:space="preserve">0.0785% </t>
         </is>
       </c>
       <c r="F45" s="2" t="n"/>
@@ -1751,22 +1791,22 @@
       </c>
       <c r="B46" s="2" t="inlineStr">
         <is>
-          <t>0x4e57abe60fdc74c47fc3a86bbd7857b4e24c180d</t>
+          <t>0x28e5d92148aa12b0fccd268ff643be86bbb5265e</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr">
         <is>
-          <t>79,763,629,301,578</t>
+          <t>75,638,511,708,227</t>
         </is>
       </c>
       <c r="D46" s="3" t="inlineStr">
         <is>
-          <t>80 Trillion</t>
+          <t>76 Trillion</t>
         </is>
       </c>
       <c r="E46" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.0798% </t>
+          <t xml:space="preserve">0.0756% </t>
         </is>
       </c>
       <c r="F46" s="2" t="n"/>
@@ -1778,22 +1818,22 @@
       </c>
       <c r="B47" s="2" t="inlineStr">
         <is>
-          <t>0xdce8e975b0dcbec956cddebffcc9f0cfaa5b8415</t>
+          <t>0xffcc995a004c26a059248c15afa92f006b315fab</t>
         </is>
       </c>
       <c r="C47" s="3" t="inlineStr">
         <is>
-          <t>78,991,697,441,408</t>
+          <t>74,204,183,091,826</t>
         </is>
       </c>
       <c r="D47" s="3" t="inlineStr">
         <is>
-          <t>79 Trillion</t>
+          <t>74 Trillion</t>
         </is>
       </c>
       <c r="E47" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.0790% </t>
+          <t xml:space="preserve">0.0742% </t>
         </is>
       </c>
       <c r="F47" s="2" t="n"/>
@@ -1805,22 +1845,22 @@
       </c>
       <c r="B48" s="2" t="inlineStr">
         <is>
-          <t>0xe902fd7de8afb5b295f628c1b4f6143005bb0bf6</t>
+          <t>0x9a7e16cc5d152e60ea52d46d8e422d724bdb4dcf</t>
         </is>
       </c>
       <c r="C48" s="3" t="inlineStr">
         <is>
-          <t>78,500,122,588,755</t>
+          <t>72,904,810,003,324</t>
         </is>
       </c>
       <c r="D48" s="3" t="inlineStr">
         <is>
-          <t>79 Trillion</t>
+          <t>73 Trillion</t>
         </is>
       </c>
       <c r="E48" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.0785% </t>
+          <t xml:space="preserve">0.0729% </t>
         </is>
       </c>
       <c r="F48" s="2" t="n"/>
@@ -1832,22 +1872,22 @@
       </c>
       <c r="B49" s="2" t="inlineStr">
         <is>
-          <t>0x28e5d92148aa12b0fccd268ff643be86bbb5265e</t>
+          <t>0x0fcb56c9e4f865e48475bab332b4e86f78332a55</t>
         </is>
       </c>
       <c r="C49" s="3" t="inlineStr">
         <is>
-          <t>75,630,491,800,321</t>
+          <t>71,201,112,114,715</t>
         </is>
       </c>
       <c r="D49" s="3" t="inlineStr">
         <is>
-          <t>76 Trillion</t>
+          <t>71 Trillion</t>
         </is>
       </c>
       <c r="E49" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.0756% </t>
+          <t xml:space="preserve">0.0712% </t>
         </is>
       </c>
       <c r="F49" s="2" t="n"/>
@@ -1861,12 +1901,12 @@
       </c>
       <c r="C51" s="3" t="inlineStr">
         <is>
-          <t>8,740,386,620,482,522</t>
+          <t>8,743,124,061,599,851</t>
         </is>
       </c>
       <c r="D51" s="3" t="inlineStr">
         <is>
-          <t>8740 Trillion</t>
+          <t>8743 Trillion</t>
         </is>
       </c>
       <c r="E51" s="3" t="inlineStr">
@@ -1876,12 +1916,12 @@
       </c>
       <c r="F51" s="2" t="inlineStr">
         <is>
-          <t>18 Trillion</t>
+          <t>64 Trillion</t>
         </is>
       </c>
       <c r="G51" s="2" t="inlineStr">
         <is>
-          <t>18,382,621,033,105</t>
+          <t>64,116,523,388,014</t>
         </is>
       </c>
     </row>
@@ -1904,32 +1944,32 @@
       </c>
       <c r="B54" s="4" t="inlineStr">
         <is>
-          <t>0x7b11f31fc0d0a79717ec025d411ac5e899ac7116</t>
+          <t>0x84d1b0ae25aa0b535552d28455f4d00922baf624</t>
         </is>
       </c>
       <c r="C54" s="5" t="inlineStr">
         <is>
-          <t>39,469,942,950,288</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D54" s="5" t="inlineStr">
         <is>
-          <t>39 Trillion</t>
+          <t>0 Trillion</t>
         </is>
       </c>
       <c r="E54" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1287% </t>
+          <t xml:space="preserve">0.1048% </t>
         </is>
       </c>
       <c r="F54" s="6" t="inlineStr">
         <is>
-          <t>89 Trillion Less</t>
+          <t>105 Trillion Less</t>
         </is>
       </c>
       <c r="G54" s="7" t="inlineStr">
         <is>
-          <t>89,257,740,169,579</t>
+          <t>104,834,199,490,524</t>
         </is>
       </c>
     </row>
@@ -1939,32 +1979,32 @@
       </c>
       <c r="B55" s="4" t="inlineStr">
         <is>
-          <t>0x74beaeb59500b4486ec3c83b81552279b79c6728</t>
+          <t>0x83cd797812ebcfe418f76a16fb15c7f149eaa2f7</t>
         </is>
       </c>
       <c r="C55" s="5" t="inlineStr">
         <is>
-          <t>12,748,538,523,985</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D55" s="5" t="inlineStr">
         <is>
-          <t>13 Trillion</t>
+          <t>0 Trillion</t>
         </is>
       </c>
       <c r="E55" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1080% </t>
+          <t xml:space="preserve">0.1138% </t>
         </is>
       </c>
       <c r="F55" s="6" t="inlineStr">
         <is>
-          <t>95 Trillion Less</t>
+          <t>114 Trillion Less</t>
         </is>
       </c>
       <c r="G55" s="7" t="inlineStr">
         <is>
-          <t>95,293,947,858,899</t>
+          <t>113,815,954,518,575</t>
         </is>
       </c>
     </row>
@@ -1974,7 +2014,7 @@
       </c>
       <c r="B56" s="4" t="inlineStr">
         <is>
-          <t>0x83cd797812ebcfe418f76a16fb15c7f149eaa2f7</t>
+          <t>0x34db618752319744a4a41e6ba4d5d58b3fffff48</t>
         </is>
       </c>
       <c r="C56" s="5" t="inlineStr">
@@ -1989,17 +2029,17 @@
       </c>
       <c r="E56" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1138% </t>
+          <t xml:space="preserve">1.0630% </t>
         </is>
       </c>
       <c r="F56" s="6" t="inlineStr">
         <is>
-          <t>114 Trillion Less</t>
+          <t>1063 Trillion Less</t>
         </is>
       </c>
       <c r="G56" s="7" t="inlineStr">
         <is>
-          <t>113,815,954,518,575</t>
+          <t>1,062,974,248,973,550</t>
         </is>
       </c>
     </row>
@@ -2009,50 +2049,120 @@
       </c>
       <c r="B57" s="4" t="inlineStr">
         <is>
-          <t>0x34db618752319744a4a41e6ba4d5d58b3fffff48</t>
+          <t>0x7b11f31fc0d0a79717ec025d411ac5e899ac7116</t>
         </is>
       </c>
       <c r="C57" s="5" t="inlineStr">
         <is>
+          <t>39,482,797,795,782</t>
+        </is>
+      </c>
+      <c r="D57" s="5" t="inlineStr">
+        <is>
+          <t>39 Trillion</t>
+        </is>
+      </c>
+      <c r="E57" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.1287% </t>
+        </is>
+      </c>
+      <c r="F57" s="6" t="inlineStr">
+        <is>
+          <t>89 Trillion Less</t>
+        </is>
+      </c>
+      <c r="G57" s="7" t="inlineStr">
+        <is>
+          <t>89,244,885,324,085</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B58" s="4" t="inlineStr">
+        <is>
+          <t>0x69fe97ce030074b37cbaf3ee46e9f68ca8712099</t>
+        </is>
+      </c>
+      <c r="C58" s="5" t="inlineStr">
+        <is>
           <t>0</t>
         </is>
       </c>
-      <c r="D57" s="5" t="inlineStr">
+      <c r="D58" s="5" t="inlineStr">
         <is>
           <t>0 Trillion</t>
         </is>
       </c>
-      <c r="E57" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">1.0630% </t>
-        </is>
-      </c>
-      <c r="F57" s="6" t="inlineStr">
-        <is>
-          <t>1063 Trillion Less</t>
-        </is>
-      </c>
-      <c r="G57" s="7" t="inlineStr">
-        <is>
-          <t>1,062,974,248,973,550</t>
+      <c r="E58" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.1006% </t>
+        </is>
+      </c>
+      <c r="F58" s="6" t="inlineStr">
+        <is>
+          <t>101 Trillion Less</t>
+        </is>
+      </c>
+      <c r="G58" s="7" t="inlineStr">
+        <is>
+          <t>100,567,579,913,450</t>
         </is>
       </c>
     </row>
     <row r="59">
-      <c r="D59" s="6" t="n"/>
-      <c r="E59" s="7" t="inlineStr">
+      <c r="A59" s="4" t="n">
+        <v>6</v>
+      </c>
+      <c r="B59" s="4" t="inlineStr">
+        <is>
+          <t>0x302c44b648f5a84191f08551be26a2d2456a1fa1</t>
+        </is>
+      </c>
+      <c r="C59" s="5" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D59" s="5" t="inlineStr">
+        <is>
+          <t>0 Trillion</t>
+        </is>
+      </c>
+      <c r="E59" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.0939% </t>
+        </is>
+      </c>
+      <c r="F59" s="6" t="inlineStr">
+        <is>
+          <t>94 Trillion Less</t>
+        </is>
+      </c>
+      <c r="G59" s="7" t="inlineStr">
+        <is>
+          <t>93,917,447,289,939</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="D61" s="6" t="n"/>
+      <c r="E61" s="7" t="inlineStr">
         <is>
           <t>Total loss / gain from all whales</t>
         </is>
       </c>
-      <c r="F59" s="6" t="inlineStr">
-        <is>
-          <t>-1343 Trillion</t>
-        </is>
-      </c>
-      <c r="G59" s="6" t="inlineStr">
-        <is>
-          <t>-1,342,959,270,487,498</t>
+      <c r="F61" s="6" t="inlineStr">
+        <is>
+          <t>-1501 Trillion</t>
+        </is>
+      </c>
+      <c r="G61" s="6" t="inlineStr">
+        <is>
+          <t>-1,501,237,792,122,109</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Just 1 more update
</commit_message>
<xml_diff>
--- a/whales/holders.xlsx
+++ b/whales/holders.xlsx
@@ -451,7 +451,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:G59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -512,7 +512,7 @@
       </c>
       <c r="C2" s="3" t="inlineStr">
         <is>
-          <t>774,216,186,127,082</t>
+          <t>774,307,561,983,887</t>
         </is>
       </c>
       <c r="D2" s="3" t="inlineStr">
@@ -522,7 +522,7 @@
       </c>
       <c r="E2" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.7742% </t>
+          <t xml:space="preserve">0.7743% </t>
         </is>
       </c>
       <c r="F2" s="2" t="n"/>
@@ -539,7 +539,7 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>608,650,037,852,732</t>
+          <t>608,708,314,713,528</t>
         </is>
       </c>
       <c r="D3" s="3" t="inlineStr">
@@ -566,7 +566,7 @@
       </c>
       <c r="C4" s="3" t="inlineStr">
         <is>
-          <t>411,090,731,506,089</t>
+          <t>411,136,520,100,173</t>
         </is>
       </c>
       <c r="D4" s="3" t="inlineStr">
@@ -593,7 +593,7 @@
       </c>
       <c r="C5" s="3" t="inlineStr">
         <is>
-          <t>409,442,720,828,911</t>
+          <t>409,488,530,063,438</t>
         </is>
       </c>
       <c r="D5" s="3" t="inlineStr">
@@ -603,7 +603,7 @@
       </c>
       <c r="E5" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.4094% </t>
+          <t xml:space="preserve">0.4095% </t>
         </is>
       </c>
       <c r="F5" s="2" t="n"/>
@@ -620,7 +620,7 @@
       </c>
       <c r="C6" s="3" t="inlineStr">
         <is>
-          <t>401,991,199,429,829</t>
+          <t>402,035,974,489,069</t>
         </is>
       </c>
       <c r="D6" s="3" t="inlineStr">
@@ -637,39 +637,31 @@
       <c r="G6" s="2" t="n"/>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="n">
+      <c r="A7" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="4" t="inlineStr">
+      <c r="B7" s="2" t="inlineStr">
         <is>
           <t>0xbd09e0594fbdbc5f73fe5db01bdc3bc2a19ec2d7</t>
         </is>
       </c>
-      <c r="C7" s="5" t="inlineStr">
-        <is>
-          <t>387,893,772,035,584</t>
-        </is>
-      </c>
-      <c r="D7" s="5" t="inlineStr">
+      <c r="C7" s="3" t="inlineStr">
+        <is>
+          <t>387,947,138,413,789</t>
+        </is>
+      </c>
+      <c r="D7" s="3" t="inlineStr">
         <is>
           <t>388 Trillion</t>
         </is>
       </c>
-      <c r="E7" s="5" t="inlineStr">
+      <c r="E7" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">0.3879% </t>
         </is>
       </c>
-      <c r="F7" s="6" t="inlineStr">
-        <is>
-          <t>30 Trillion Less</t>
-        </is>
-      </c>
-      <c r="G7" s="7" t="inlineStr">
-        <is>
-          <t>29,983,511,181,832</t>
-        </is>
-      </c>
+      <c r="F7" s="2" t="n"/>
+      <c r="G7" s="2" t="n"/>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
@@ -682,7 +674,7 @@
       </c>
       <c r="C8" s="3" t="inlineStr">
         <is>
-          <t>375,131,643,268,213</t>
+          <t>375,177,377,698,958</t>
         </is>
       </c>
       <c r="D8" s="3" t="inlineStr">
@@ -692,7 +684,7 @@
       </c>
       <c r="E8" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.3751% </t>
+          <t xml:space="preserve">0.3752% </t>
         </is>
       </c>
       <c r="F8" s="2" t="n"/>
@@ -709,7 +701,7 @@
       </c>
       <c r="C9" s="5" t="inlineStr">
         <is>
-          <t>316,311,829,818,156</t>
+          <t>316,360,694,942,706</t>
         </is>
       </c>
       <c r="D9" s="5" t="inlineStr">
@@ -719,17 +711,17 @@
       </c>
       <c r="E9" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.3163% </t>
+          <t xml:space="preserve">0.3164% </t>
         </is>
       </c>
       <c r="F9" s="4" t="inlineStr">
         <is>
-          <t>10 Trillion More</t>
+          <t>5 Trillion More</t>
         </is>
       </c>
       <c r="G9" s="5" t="inlineStr">
         <is>
-          <t>9,932,087,203,919</t>
+          <t>4,970,726,217,924</t>
         </is>
       </c>
     </row>
@@ -761,74 +753,58 @@
       <c r="G10" s="2" t="n"/>
     </row>
     <row r="11">
-      <c r="A11" s="4" t="n">
+      <c r="A11" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="4" t="inlineStr">
+      <c r="B11" s="2" t="inlineStr">
         <is>
           <t>0xfdd50de023c9a705d9086bf821d15c7450ee93bf</t>
         </is>
       </c>
-      <c r="C11" s="5" t="inlineStr">
+      <c r="C11" s="3" t="inlineStr">
         <is>
           <t>227,648,398,367,749</t>
         </is>
       </c>
-      <c r="D11" s="5" t="inlineStr">
+      <c r="D11" s="3" t="inlineStr">
         <is>
           <t>228 Trillion</t>
         </is>
       </c>
-      <c r="E11" s="5" t="inlineStr">
+      <c r="E11" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">0.2276% </t>
         </is>
       </c>
-      <c r="F11" s="4" t="inlineStr">
-        <is>
-          <t>1 Trillion More</t>
-        </is>
-      </c>
-      <c r="G11" s="5" t="inlineStr">
-        <is>
-          <t>1,153,143,662,657</t>
-        </is>
-      </c>
+      <c r="F11" s="2" t="n"/>
+      <c r="G11" s="2" t="n"/>
     </row>
     <row r="12">
-      <c r="A12" s="4" t="n">
+      <c r="A12" s="2" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="inlineStr">
+      <c r="B12" s="2" t="inlineStr">
         <is>
           <t>0x112344b8882619f5c8cfa9901d0b88e9eb11a25a</t>
         </is>
       </c>
-      <c r="C12" s="5" t="inlineStr">
-        <is>
-          <t>200,307,986,170,445</t>
-        </is>
-      </c>
-      <c r="D12" s="5" t="inlineStr">
+      <c r="C12" s="3" t="inlineStr">
+        <is>
+          <t>200,329,664,061,462</t>
+        </is>
+      </c>
+      <c r="D12" s="3" t="inlineStr">
         <is>
           <t>200 Trillion</t>
         </is>
       </c>
-      <c r="E12" s="5" t="inlineStr">
+      <c r="E12" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">0.2003% </t>
         </is>
       </c>
-      <c r="F12" s="4" t="inlineStr">
-        <is>
-          <t>14 Trillion More</t>
-        </is>
-      </c>
-      <c r="G12" s="5" t="inlineStr">
-        <is>
-          <t>14,261,131,020,044</t>
-        </is>
-      </c>
+      <c r="F12" s="2" t="n"/>
+      <c r="G12" s="2" t="n"/>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
@@ -841,7 +817,7 @@
       </c>
       <c r="C13" s="3" t="inlineStr">
         <is>
-          <t>190,593,752,012,968</t>
+          <t>190,701,478,480,220</t>
         </is>
       </c>
       <c r="D13" s="3" t="inlineStr">
@@ -851,7 +827,7 @@
       </c>
       <c r="E13" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1906% </t>
+          <t xml:space="preserve">0.1907% </t>
         </is>
       </c>
       <c r="F13" s="2" t="n"/>
@@ -868,7 +844,7 @@
       </c>
       <c r="C14" s="3" t="inlineStr">
         <is>
-          <t>188,093,487,682,416</t>
+          <t>188,199,784,143,419</t>
         </is>
       </c>
       <c r="D14" s="3" t="inlineStr">
@@ -878,7 +854,7 @@
       </c>
       <c r="E14" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1881% </t>
+          <t xml:space="preserve">0.1882% </t>
         </is>
       </c>
       <c r="F14" s="2" t="n"/>
@@ -895,7 +871,7 @@
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>180,049,748,547,878</t>
+          <t>180,061,685,729,809</t>
         </is>
       </c>
       <c r="D15" s="5" t="inlineStr">
@@ -905,7 +881,7 @@
       </c>
       <c r="E15" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1800% </t>
+          <t xml:space="preserve">0.1801% </t>
         </is>
       </c>
       <c r="F15" s="6" t="inlineStr">
@@ -915,7 +891,7 @@
       </c>
       <c r="G15" s="7" t="inlineStr">
         <is>
-          <t>16,708,711,049,687</t>
+          <t>16,849,757,130,762</t>
         </is>
       </c>
     </row>
@@ -930,7 +906,7 @@
       </c>
       <c r="C16" s="3" t="inlineStr">
         <is>
-          <t>174,420,634,860,359</t>
+          <t>174,442,294,351,054</t>
         </is>
       </c>
       <c r="D16" s="3" t="inlineStr">
@@ -974,66 +950,66 @@
       <c r="G17" s="2" t="n"/>
     </row>
     <row r="18">
-      <c r="A18" s="4" t="n">
+      <c r="A18" s="2" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="4" t="inlineStr">
+      <c r="B18" s="2" t="inlineStr">
         <is>
           <t>0xb05a41293daf0fa7c71e4e035e2f477299fe10a1</t>
         </is>
       </c>
-      <c r="C18" s="5" t="inlineStr">
+      <c r="C18" s="3" t="inlineStr">
         <is>
           <t>161,527,403,951,616</t>
         </is>
       </c>
-      <c r="D18" s="5" t="inlineStr">
+      <c r="D18" s="3" t="inlineStr">
         <is>
           <t>162 Trillion</t>
         </is>
       </c>
-      <c r="E18" s="5" t="inlineStr">
+      <c r="E18" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">0.1615% </t>
         </is>
       </c>
-      <c r="F18" s="4" t="inlineStr">
-        <is>
-          <t>51 Trillion More</t>
-        </is>
-      </c>
-      <c r="G18" s="5" t="inlineStr">
-        <is>
-          <t>51,009,307,857,513</t>
-        </is>
-      </c>
+      <c r="F18" s="2" t="n"/>
+      <c r="G18" s="2" t="n"/>
     </row>
     <row r="19">
-      <c r="A19" s="2" t="n">
+      <c r="A19" s="4" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="2" t="inlineStr">
-        <is>
-          <t>0x7b5b9b8d134bec76023cd6c20358d38714cc5c58</t>
-        </is>
-      </c>
-      <c r="C19" s="3" t="inlineStr">
-        <is>
-          <t>154,509,886,822,012</t>
-        </is>
-      </c>
-      <c r="D19" s="3" t="inlineStr">
-        <is>
-          <t>155 Trillion</t>
-        </is>
-      </c>
-      <c r="E19" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.1545% </t>
-        </is>
-      </c>
-      <c r="F19" s="2" t="n"/>
-      <c r="G19" s="2" t="n"/>
+      <c r="B19" s="4" t="inlineStr">
+        <is>
+          <t>0xf08ae27b3b1c31d1cfc2879e2ae567d81d42bdeb</t>
+        </is>
+      </c>
+      <c r="C19" s="5" t="inlineStr">
+        <is>
+          <t>156,883,028,878,428</t>
+        </is>
+      </c>
+      <c r="D19" s="5" t="inlineStr">
+        <is>
+          <t>157 Trillion</t>
+        </is>
+      </c>
+      <c r="E19" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.1569% </t>
+        </is>
+      </c>
+      <c r="F19" s="4" t="inlineStr">
+        <is>
+          <t>11 Trillion More</t>
+        </is>
+      </c>
+      <c r="G19" s="5" t="inlineStr">
+        <is>
+          <t>10,802,619,956,627</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
@@ -1041,123 +1017,115 @@
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
-          <t>0x1ae48253b364374d3db52de311302fc501b87895</t>
+          <t>0x7b5b9b8d134bec76023cd6c20358d38714cc5c58</t>
         </is>
       </c>
       <c r="C20" s="3" t="inlineStr">
         <is>
-          <t>153,700,859,113,465</t>
+          <t>154,659,042,382,428</t>
         </is>
       </c>
       <c r="D20" s="3" t="inlineStr">
         <is>
-          <t>154 Trillion</t>
+          <t>155 Trillion</t>
         </is>
       </c>
       <c r="E20" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1537% </t>
+          <t xml:space="preserve">0.1547% </t>
         </is>
       </c>
       <c r="F20" s="2" t="n"/>
       <c r="G20" s="2" t="n"/>
     </row>
     <row r="21">
-      <c r="A21" s="4" t="n">
+      <c r="A21" s="2" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="4" t="inlineStr">
+      <c r="B21" s="2" t="inlineStr">
+        <is>
+          <t>0x1ae48253b364374d3db52de311302fc501b87895</t>
+        </is>
+      </c>
+      <c r="C21" s="3" t="inlineStr">
+        <is>
+          <t>153,720,855,176,997</t>
+        </is>
+      </c>
+      <c r="D21" s="3" t="inlineStr">
+        <is>
+          <t>154 Trillion</t>
+        </is>
+      </c>
+      <c r="E21" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.1537% </t>
+        </is>
+      </c>
+      <c r="F21" s="2" t="n"/>
+      <c r="G21" s="2" t="n"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="inlineStr">
         <is>
           <t>0x497e289791fc2c2b355c259d9516f079d9b52a63</t>
         </is>
       </c>
-      <c r="C21" s="5" t="inlineStr">
-        <is>
-          <t>151,329,188,545,567</t>
-        </is>
-      </c>
-      <c r="D21" s="5" t="inlineStr">
+      <c r="C22" s="3" t="inlineStr">
+        <is>
+          <t>151,369,585,024,300</t>
+        </is>
+      </c>
+      <c r="D22" s="3" t="inlineStr">
         <is>
           <t>151 Trillion</t>
         </is>
       </c>
-      <c r="E21" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.1513% </t>
-        </is>
-      </c>
-      <c r="F21" s="6" t="inlineStr">
-        <is>
-          <t>29 Trillion Less</t>
-        </is>
-      </c>
-      <c r="G21" s="7" t="inlineStr">
-        <is>
-          <t>28,720,318,521,664</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="4" t="n">
-        <v>21</v>
-      </c>
-      <c r="B22" s="4" t="inlineStr">
+      <c r="E22" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.1514% </t>
+        </is>
+      </c>
+      <c r="F22" s="2" t="n"/>
+      <c r="G22" s="2" t="n"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="4" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="4" t="inlineStr">
         <is>
           <t>0x4ac84bbb674f62614626f6276296014f1cade575</t>
         </is>
       </c>
-      <c r="C22" s="5" t="inlineStr">
-        <is>
-          <t>148,109,255,191,595</t>
-        </is>
-      </c>
-      <c r="D22" s="5" t="inlineStr">
-        <is>
-          <t>148 Trillion</t>
-        </is>
-      </c>
-      <c r="E22" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.1481% </t>
-        </is>
-      </c>
-      <c r="F22" s="4" t="inlineStr">
-        <is>
-          <t>7 Trillion More</t>
-        </is>
-      </c>
-      <c r="G22" s="5" t="inlineStr">
-        <is>
-          <t>6,846,266,779,468</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="2" t="n">
-        <v>22</v>
-      </c>
-      <c r="B23" s="2" t="inlineStr">
-        <is>
-          <t>0xf08ae27b3b1c31d1cfc2879e2ae567d81d42bdeb</t>
-        </is>
-      </c>
-      <c r="C23" s="3" t="inlineStr">
-        <is>
-          <t>146,185,236,267,846</t>
-        </is>
-      </c>
-      <c r="D23" s="3" t="inlineStr">
-        <is>
-          <t>146 Trillion</t>
-        </is>
-      </c>
-      <c r="E23" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.1462% </t>
-        </is>
-      </c>
-      <c r="F23" s="2" t="n"/>
-      <c r="G23" s="2" t="n"/>
+      <c r="C23" s="5" t="inlineStr">
+        <is>
+          <t>149,569,810,762,960</t>
+        </is>
+      </c>
+      <c r="D23" s="5" t="inlineStr">
+        <is>
+          <t>150 Trillion</t>
+        </is>
+      </c>
+      <c r="E23" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.1496% </t>
+        </is>
+      </c>
+      <c r="F23" s="4" t="inlineStr">
+        <is>
+          <t>8 Trillion More</t>
+        </is>
+      </c>
+      <c r="G23" s="5" t="inlineStr">
+        <is>
+          <t>8,194,009,460,942</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
@@ -1187,39 +1155,31 @@
       <c r="G24" s="2" t="n"/>
     </row>
     <row r="25">
-      <c r="A25" s="4" t="n">
+      <c r="A25" s="2" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="4" t="inlineStr">
+      <c r="B25" s="2" t="inlineStr">
         <is>
           <t>0x74beaeb59500b4486ec3c83b81552279b79c6728</t>
         </is>
       </c>
-      <c r="C25" s="5" t="inlineStr">
+      <c r="C25" s="3" t="inlineStr">
         <is>
           <t>134,413,919,604,666</t>
         </is>
       </c>
-      <c r="D25" s="5" t="inlineStr">
+      <c r="D25" s="3" t="inlineStr">
         <is>
           <t>134 Trillion</t>
         </is>
       </c>
-      <c r="E25" s="5" t="inlineStr">
+      <c r="E25" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">0.1344% </t>
         </is>
       </c>
-      <c r="F25" s="4" t="inlineStr">
-        <is>
-          <t>26 Trillion More</t>
-        </is>
-      </c>
-      <c r="G25" s="5" t="inlineStr">
-        <is>
-          <t>26,371,433,221,782</t>
-        </is>
-      </c>
+      <c r="F25" s="2" t="n"/>
+      <c r="G25" s="2" t="n"/>
     </row>
     <row r="26">
       <c r="A26" s="4" t="n">
@@ -1365,39 +1325,31 @@
       <c r="G30" s="2" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" s="4" t="n">
+      <c r="A31" s="2" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="4" t="inlineStr">
+      <c r="B31" s="2" t="inlineStr">
         <is>
           <t>0x2fcc0ac77971df25d65b9eae9418434ac72be3bc</t>
         </is>
       </c>
-      <c r="C31" s="5" t="inlineStr">
+      <c r="C31" s="3" t="inlineStr">
         <is>
           <t>108,170,757,830,871</t>
         </is>
       </c>
-      <c r="D31" s="5" t="inlineStr">
+      <c r="D31" s="3" t="inlineStr">
         <is>
           <t>108 Trillion</t>
         </is>
       </c>
-      <c r="E31" s="5" t="inlineStr">
+      <c r="E31" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve">0.1082% </t>
         </is>
       </c>
-      <c r="F31" s="4" t="inlineStr">
-        <is>
-          <t>6 Trillion More</t>
-        </is>
-      </c>
-      <c r="G31" s="5" t="inlineStr">
-        <is>
-          <t>5,951,202,366,611</t>
-        </is>
-      </c>
+      <c r="F31" s="2" t="n"/>
+      <c r="G31" s="2" t="n"/>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
@@ -1513,22 +1465,22 @@
       </c>
       <c r="B36" s="2" t="inlineStr">
         <is>
-          <t>0xe7af2280c3a70170f9e5cb67c6ea5885680d2838</t>
+          <t>0x0fcb56c9e4f865e48475bab332b4e86f78332a55</t>
         </is>
       </c>
       <c r="C36" s="3" t="inlineStr">
         <is>
-          <t>101,057,958,101,905</t>
+          <t>101,595,431,794,851</t>
         </is>
       </c>
       <c r="D36" s="3" t="inlineStr">
         <is>
-          <t>101 Trillion</t>
+          <t>102 Trillion</t>
         </is>
       </c>
       <c r="E36" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1011% </t>
+          <t xml:space="preserve">0.1016% </t>
         </is>
       </c>
       <c r="F36" s="2" t="n"/>
@@ -1540,22 +1492,22 @@
       </c>
       <c r="B37" s="2" t="inlineStr">
         <is>
-          <t>0xa9579390b4b5ac986a16a05c32ad0975e089a857</t>
+          <t>0xe7af2280c3a70170f9e5cb67c6ea5885680d2838</t>
         </is>
       </c>
       <c r="C37" s="3" t="inlineStr">
         <is>
-          <t>100,126,359,859,271</t>
+          <t>101,057,958,101,905</t>
         </is>
       </c>
       <c r="D37" s="3" t="inlineStr">
         <is>
-          <t>100 Trillion</t>
+          <t>101 Trillion</t>
         </is>
       </c>
       <c r="E37" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1001% </t>
+          <t xml:space="preserve">0.1011% </t>
         </is>
       </c>
       <c r="F37" s="2" t="n"/>
@@ -1567,53 +1519,61 @@
       </c>
       <c r="B38" s="2" t="inlineStr">
         <is>
-          <t>0x021bcf7b581b6328c458f13ebb50ea6767c1b16d</t>
+          <t>0xa9579390b4b5ac986a16a05c32ad0975e089a857</t>
         </is>
       </c>
       <c r="C38" s="3" t="inlineStr">
         <is>
-          <t>92,888,524,562,195</t>
+          <t>100,126,359,859,271</t>
         </is>
       </c>
       <c r="D38" s="3" t="inlineStr">
         <is>
-          <t>93 Trillion</t>
+          <t>100 Trillion</t>
         </is>
       </c>
       <c r="E38" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.0929% </t>
+          <t xml:space="preserve">0.1001% </t>
         </is>
       </c>
       <c r="F38" s="2" t="n"/>
       <c r="G38" s="2" t="n"/>
     </row>
     <row r="39">
-      <c r="A39" s="2" t="n">
+      <c r="A39" s="4" t="n">
         <v>38</v>
       </c>
-      <c r="B39" s="2" t="inlineStr">
-        <is>
-          <t>0xf8a002718fbba65dd1ca19e7027c943c54e20220</t>
-        </is>
-      </c>
-      <c r="C39" s="3" t="inlineStr">
-        <is>
-          <t>90,569,119,873,037</t>
-        </is>
-      </c>
-      <c r="D39" s="3" t="inlineStr">
-        <is>
-          <t>91 Trillion</t>
-        </is>
-      </c>
-      <c r="E39" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.0906% </t>
-        </is>
-      </c>
-      <c r="F39" s="2" t="n"/>
-      <c r="G39" s="2" t="n"/>
+      <c r="B39" s="4" t="inlineStr">
+        <is>
+          <t>0x021bcf7b581b6328c458f13ebb50ea6767c1b16d</t>
+        </is>
+      </c>
+      <c r="C39" s="5" t="inlineStr">
+        <is>
+          <t>92,888,524,562,195</t>
+        </is>
+      </c>
+      <c r="D39" s="5" t="inlineStr">
+        <is>
+          <t>93 Trillion</t>
+        </is>
+      </c>
+      <c r="E39" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.0929% </t>
+        </is>
+      </c>
+      <c r="F39" s="4" t="inlineStr">
+        <is>
+          <t>7 Trillion More</t>
+        </is>
+      </c>
+      <c r="G39" s="5" t="inlineStr">
+        <is>
+          <t>7,475,885,161,112</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="n">
@@ -1621,88 +1581,88 @@
       </c>
       <c r="B40" s="2" t="inlineStr">
         <is>
-          <t>0xb501e46d0e187cd9e2e0b3611fe17ed477f998e1</t>
+          <t>0xf8a002718fbba65dd1ca19e7027c943c54e20220</t>
         </is>
       </c>
       <c r="C40" s="3" t="inlineStr">
         <is>
-          <t>87,819,801,364,648</t>
+          <t>90,579,859,718,540</t>
         </is>
       </c>
       <c r="D40" s="3" t="inlineStr">
         <is>
-          <t>88 Trillion</t>
+          <t>91 Trillion</t>
         </is>
       </c>
       <c r="E40" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.0878% </t>
+          <t xml:space="preserve">0.0906% </t>
         </is>
       </c>
       <c r="F40" s="2" t="n"/>
       <c r="G40" s="2" t="n"/>
     </row>
     <row r="41">
-      <c r="A41" s="4" t="n">
+      <c r="A41" s="2" t="n">
         <v>40</v>
       </c>
-      <c r="B41" s="4" t="inlineStr">
+      <c r="B41" s="2" t="inlineStr">
+        <is>
+          <t>0xb501e46d0e187cd9e2e0b3611fe17ed477f998e1</t>
+        </is>
+      </c>
+      <c r="C41" s="3" t="inlineStr">
+        <is>
+          <t>87,819,801,364,648</t>
+        </is>
+      </c>
+      <c r="D41" s="3" t="inlineStr">
+        <is>
+          <t>88 Trillion</t>
+        </is>
+      </c>
+      <c r="E41" s="3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">0.0878% </t>
+        </is>
+      </c>
+      <c r="F41" s="2" t="n"/>
+      <c r="G41" s="2" t="n"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="4" t="n">
+        <v>41</v>
+      </c>
+      <c r="B42" s="4" t="inlineStr">
         <is>
           <t>0xd8f8110161649178bca78b074cef0864ad9a99a8</t>
         </is>
       </c>
-      <c r="C41" s="5" t="inlineStr">
-        <is>
-          <t>87,159,029,085,616</t>
-        </is>
-      </c>
-      <c r="D41" s="5" t="inlineStr">
+      <c r="C42" s="5" t="inlineStr">
+        <is>
+          <t>87,170,129,309,799</t>
+        </is>
+      </c>
+      <c r="D42" s="5" t="inlineStr">
         <is>
           <t>87 Trillion</t>
         </is>
       </c>
-      <c r="E41" s="5" t="inlineStr">
+      <c r="E42" s="5" t="inlineStr">
         <is>
           <t xml:space="preserve">0.0872% </t>
         </is>
       </c>
-      <c r="F41" s="4" t="inlineStr">
+      <c r="F42" s="4" t="inlineStr">
         <is>
           <t>4 Trillion More</t>
         </is>
       </c>
-      <c r="G41" s="5" t="inlineStr">
-        <is>
-          <t>4,243,865,932,513</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="2" t="n">
-        <v>41</v>
-      </c>
-      <c r="B42" s="2" t="inlineStr">
-        <is>
-          <t>0xca1135931ecedc74d402c712678d555286c6dbf8</t>
-        </is>
-      </c>
-      <c r="C42" s="3" t="inlineStr">
-        <is>
-          <t>86,961,842,948,968</t>
-        </is>
-      </c>
-      <c r="D42" s="3" t="inlineStr">
-        <is>
-          <t>87 Trillion</t>
-        </is>
-      </c>
-      <c r="E42" s="3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.0870% </t>
-        </is>
-      </c>
-      <c r="F42" s="2" t="n"/>
-      <c r="G42" s="2" t="n"/>
+      <c r="G42" s="5" t="inlineStr">
+        <is>
+          <t>4,210,279,168,027</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="n">
@@ -1710,22 +1670,22 @@
       </c>
       <c r="B43" s="2" t="inlineStr">
         <is>
-          <t>0xa6864e154b64a8ce94020a8c1b43f191d3523c47</t>
+          <t>0xca1135931ecedc74d402c712678d555286c6dbf8</t>
         </is>
       </c>
       <c r="C43" s="3" t="inlineStr">
         <is>
-          <t>81,128,791,830,716</t>
+          <t>86,961,842,948,968</t>
         </is>
       </c>
       <c r="D43" s="3" t="inlineStr">
         <is>
-          <t>81 Trillion</t>
+          <t>87 Trillion</t>
         </is>
       </c>
       <c r="E43" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.0811% </t>
+          <t xml:space="preserve">0.0870% </t>
         </is>
       </c>
       <c r="F43" s="2" t="n"/>
@@ -1737,22 +1697,22 @@
       </c>
       <c r="B44" s="2" t="inlineStr">
         <is>
-          <t>0x4e57abe60fdc74c47fc3a86bbd7857b4e24c180d</t>
+          <t>0xa6864e154b64a8ce94020a8c1b43f191d3523c47</t>
         </is>
       </c>
       <c r="C44" s="3" t="inlineStr">
         <is>
-          <t>79,763,629,301,578</t>
+          <t>81,128,791,830,716</t>
         </is>
       </c>
       <c r="D44" s="3" t="inlineStr">
         <is>
-          <t>80 Trillion</t>
+          <t>81 Trillion</t>
         </is>
       </c>
       <c r="E44" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.0798% </t>
+          <t xml:space="preserve">0.0811% </t>
         </is>
       </c>
       <c r="F44" s="2" t="n"/>
@@ -1764,22 +1724,22 @@
       </c>
       <c r="B45" s="2" t="inlineStr">
         <is>
-          <t>0xe902fd7de8afb5b295f628c1b4f6143005bb0bf6</t>
+          <t>0x4e57abe60fdc74c47fc3a86bbd7857b4e24c180d</t>
         </is>
       </c>
       <c r="C45" s="3" t="inlineStr">
         <is>
-          <t>78,500,122,588,755</t>
+          <t>79,763,629,301,578</t>
         </is>
       </c>
       <c r="D45" s="3" t="inlineStr">
         <is>
-          <t>79 Trillion</t>
+          <t>80 Trillion</t>
         </is>
       </c>
       <c r="E45" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.0785% </t>
+          <t xml:space="preserve">0.0798% </t>
         </is>
       </c>
       <c r="F45" s="2" t="n"/>
@@ -1791,22 +1751,22 @@
       </c>
       <c r="B46" s="2" t="inlineStr">
         <is>
-          <t>0x28e5d92148aa12b0fccd268ff643be86bbb5265e</t>
+          <t>0xe902fd7de8afb5b295f628c1b4f6143005bb0bf6</t>
         </is>
       </c>
       <c r="C46" s="3" t="inlineStr">
         <is>
-          <t>75,638,511,708,227</t>
+          <t>78,500,122,588,755</t>
         </is>
       </c>
       <c r="D46" s="3" t="inlineStr">
         <is>
-          <t>76 Trillion</t>
+          <t>79 Trillion</t>
         </is>
       </c>
       <c r="E46" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.0756% </t>
+          <t xml:space="preserve">0.0785% </t>
         </is>
       </c>
       <c r="F46" s="2" t="n"/>
@@ -1818,22 +1778,22 @@
       </c>
       <c r="B47" s="2" t="inlineStr">
         <is>
-          <t>0xffcc995a004c26a059248c15afa92f006b315fab</t>
+          <t>0x28e5d92148aa12b0fccd268ff643be86bbb5265e</t>
         </is>
       </c>
       <c r="C47" s="3" t="inlineStr">
         <is>
-          <t>74,204,183,091,826</t>
+          <t>75,638,511,708,227</t>
         </is>
       </c>
       <c r="D47" s="3" t="inlineStr">
         <is>
-          <t>74 Trillion</t>
+          <t>76 Trillion</t>
         </is>
       </c>
       <c r="E47" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.0742% </t>
+          <t xml:space="preserve">0.0756% </t>
         </is>
       </c>
       <c r="F47" s="2" t="n"/>
@@ -1845,22 +1805,22 @@
       </c>
       <c r="B48" s="2" t="inlineStr">
         <is>
-          <t>0x9a7e16cc5d152e60ea52d46d8e422d724bdb4dcf</t>
+          <t>0xffcc995a004c26a059248c15afa92f006b315fab</t>
         </is>
       </c>
       <c r="C48" s="3" t="inlineStr">
         <is>
-          <t>72,904,810,003,324</t>
+          <t>74,204,183,091,826</t>
         </is>
       </c>
       <c r="D48" s="3" t="inlineStr">
         <is>
-          <t>73 Trillion</t>
+          <t>74 Trillion</t>
         </is>
       </c>
       <c r="E48" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.0729% </t>
+          <t xml:space="preserve">0.0742% </t>
         </is>
       </c>
       <c r="F48" s="2" t="n"/>
@@ -1872,22 +1832,22 @@
       </c>
       <c r="B49" s="2" t="inlineStr">
         <is>
-          <t>0x0fcb56c9e4f865e48475bab332b4e86f78332a55</t>
+          <t>0x9a7e16cc5d152e60ea52d46d8e422d724bdb4dcf</t>
         </is>
       </c>
       <c r="C49" s="3" t="inlineStr">
         <is>
-          <t>71,201,112,114,715</t>
+          <t>72,945,667,648,778</t>
         </is>
       </c>
       <c r="D49" s="3" t="inlineStr">
         <is>
-          <t>71 Trillion</t>
+          <t>73 Trillion</t>
         </is>
       </c>
       <c r="E49" s="3" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.0712% </t>
+          <t xml:space="preserve">0.0729% </t>
         </is>
       </c>
       <c r="F49" s="2" t="n"/>
@@ -1901,27 +1861,27 @@
       </c>
       <c r="C51" s="3" t="inlineStr">
         <is>
-          <t>8,743,124,061,599,851</t>
+          <t>8,786,652,264,310,605</t>
         </is>
       </c>
       <c r="D51" s="3" t="inlineStr">
         <is>
-          <t>8743 Trillion</t>
+          <t>8787 Trillion</t>
         </is>
       </c>
       <c r="E51" s="3" t="inlineStr">
         <is>
-          <t>8.74%</t>
+          <t>8.79%</t>
         </is>
       </c>
       <c r="F51" s="2" t="inlineStr">
         <is>
-          <t>64 Trillion</t>
+          <t>39 Trillion</t>
         </is>
       </c>
       <c r="G51" s="2" t="inlineStr">
         <is>
-          <t>64,116,523,388,014</t>
+          <t>38,564,388,930,560</t>
         </is>
       </c>
     </row>
@@ -1944,32 +1904,32 @@
       </c>
       <c r="B54" s="4" t="inlineStr">
         <is>
-          <t>0x84d1b0ae25aa0b535552d28455f4d00922baf624</t>
+          <t>0xdce8e975b0dcbec956cddebffcc9f0cfaa5b8415</t>
         </is>
       </c>
       <c r="C54" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>67,737,824,526,138</t>
         </is>
       </c>
       <c r="D54" s="5" t="inlineStr">
         <is>
-          <t>0 Trillion</t>
+          <t>68 Trillion</t>
         </is>
       </c>
       <c r="E54" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1048% </t>
+          <t xml:space="preserve">0.0790% </t>
         </is>
       </c>
       <c r="F54" s="6" t="inlineStr">
         <is>
-          <t>105 Trillion Less</t>
+          <t>11 Trillion Less</t>
         </is>
       </c>
       <c r="G54" s="7" t="inlineStr">
         <is>
-          <t>104,834,199,490,524</t>
+          <t>11,253,872,915,270</t>
         </is>
       </c>
     </row>
@@ -1979,7 +1939,7 @@
       </c>
       <c r="B55" s="4" t="inlineStr">
         <is>
-          <t>0x83cd797812ebcfe418f76a16fb15c7f149eaa2f7</t>
+          <t>0x84d1b0ae25aa0b535552d28455f4d00922baf624</t>
         </is>
       </c>
       <c r="C55" s="5" t="inlineStr">
@@ -1994,17 +1954,17 @@
       </c>
       <c r="E55" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1138% </t>
+          <t xml:space="preserve">0.1048% </t>
         </is>
       </c>
       <c r="F55" s="6" t="inlineStr">
         <is>
-          <t>114 Trillion Less</t>
+          <t>105 Trillion Less</t>
         </is>
       </c>
       <c r="G55" s="7" t="inlineStr">
         <is>
-          <t>113,815,954,518,575</t>
+          <t>104,834,199,490,524</t>
         </is>
       </c>
     </row>
@@ -2014,7 +1974,7 @@
       </c>
       <c r="B56" s="4" t="inlineStr">
         <is>
-          <t>0x34db618752319744a4a41e6ba4d5d58b3fffff48</t>
+          <t>0x69fe97ce030074b37cbaf3ee46e9f68ca8712099</t>
         </is>
       </c>
       <c r="C56" s="5" t="inlineStr">
@@ -2029,17 +1989,17 @@
       </c>
       <c r="E56" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">1.0630% </t>
+          <t xml:space="preserve">0.1006% </t>
         </is>
       </c>
       <c r="F56" s="6" t="inlineStr">
         <is>
-          <t>1063 Trillion Less</t>
+          <t>101 Trillion Less</t>
         </is>
       </c>
       <c r="G56" s="7" t="inlineStr">
         <is>
-          <t>1,062,974,248,973,550</t>
+          <t>100,567,579,913,450</t>
         </is>
       </c>
     </row>
@@ -2049,120 +2009,50 @@
       </c>
       <c r="B57" s="4" t="inlineStr">
         <is>
-          <t>0x7b11f31fc0d0a79717ec025d411ac5e899ac7116</t>
+          <t>0x302c44b648f5a84191f08551be26a2d2456a1fa1</t>
         </is>
       </c>
       <c r="C57" s="5" t="inlineStr">
         <is>
-          <t>39,482,797,795,782</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D57" s="5" t="inlineStr">
         <is>
-          <t>39 Trillion</t>
+          <t>0 Trillion</t>
         </is>
       </c>
       <c r="E57" s="5" t="inlineStr">
         <is>
-          <t xml:space="preserve">0.1287% </t>
+          <t xml:space="preserve">0.0939% </t>
         </is>
       </c>
       <c r="F57" s="6" t="inlineStr">
         <is>
-          <t>89 Trillion Less</t>
+          <t>94 Trillion Less</t>
         </is>
       </c>
       <c r="G57" s="7" t="inlineStr">
         <is>
-          <t>89,244,885,324,085</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="B58" s="4" t="inlineStr">
-        <is>
-          <t>0x69fe97ce030074b37cbaf3ee46e9f68ca8712099</t>
-        </is>
-      </c>
-      <c r="C58" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D58" s="5" t="inlineStr">
-        <is>
-          <t>0 Trillion</t>
-        </is>
-      </c>
-      <c r="E58" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.1006% </t>
-        </is>
-      </c>
-      <c r="F58" s="6" t="inlineStr">
-        <is>
-          <t>101 Trillion Less</t>
-        </is>
-      </c>
-      <c r="G58" s="7" t="inlineStr">
-        <is>
-          <t>100,567,579,913,450</t>
+          <t>93,917,447,289,939</t>
         </is>
       </c>
     </row>
     <row r="59">
-      <c r="A59" s="4" t="n">
-        <v>6</v>
-      </c>
-      <c r="B59" s="4" t="inlineStr">
-        <is>
-          <t>0x302c44b648f5a84191f08551be26a2d2456a1fa1</t>
-        </is>
-      </c>
-      <c r="C59" s="5" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
-      </c>
-      <c r="D59" s="5" t="inlineStr">
-        <is>
-          <t>0 Trillion</t>
-        </is>
-      </c>
-      <c r="E59" s="5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">0.0939% </t>
+      <c r="D59" s="6" t="n"/>
+      <c r="E59" s="7" t="inlineStr">
+        <is>
+          <t>Total loss / gain from all whales</t>
         </is>
       </c>
       <c r="F59" s="6" t="inlineStr">
         <is>
-          <t>94 Trillion Less</t>
-        </is>
-      </c>
-      <c r="G59" s="7" t="inlineStr">
-        <is>
-          <t>93,917,447,289,939</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="D61" s="6" t="n"/>
-      <c r="E61" s="7" t="inlineStr">
-        <is>
-          <t>Total loss / gain from all whales</t>
-        </is>
-      </c>
-      <c r="F61" s="6" t="inlineStr">
-        <is>
-          <t>-1501 Trillion</t>
-        </is>
-      </c>
-      <c r="G61" s="6" t="inlineStr">
-        <is>
-          <t>-1,501,237,792,122,109</t>
+          <t>-272 Trillion</t>
+        </is>
+      </c>
+      <c r="G59" s="6" t="inlineStr">
+        <is>
+          <t>-272,008,710,678,623</t>
         </is>
       </c>
     </row>

</xml_diff>